<commit_message>
Add Project Schedules, qinglish MOST instructions, and revised Project Concept Note (PCN) document to replace the old MOST PCN document
Refreshed the document directory to add the following documents:

13th Five Year Plan (DRAFT 20151103) - Requirements Management.xlsx
13th Five Year Plan (DRAFT 20151103).docx
Business Planning v0.1.fts
Concept Note - Blockchain Infrastructure, Applications, and
Eco-Systems.docx
Grant Proposal Development v0.1.fts
Investment Brochure - Blockchain.pptx
MOST Basic Information Table 项目建议基本信息表.doc
MOST Project Proposal 项目建议书.doc
Municipal Distributed Ledger Development Platform v0.1 Implementation
Schedule.fts
Project Concept Note (PCN) – Municipal Distributed Ledger Pilot
Development Platform for All Economic Activities.docx
UNIDO Feasibility Study Report v0.1.fts
</commit_message>
<xml_diff>
--- a/13th Five Year Plan (DRAFT 20151103) - Requirements Management.xlsx
+++ b/13th Five Year Plan (DRAFT 20151103) - Requirements Management.xlsx
@@ -1383,12 +1383,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1410,14 +1404,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1705,11 +1705,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="67.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1717,23 +1717,23 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="70" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="70" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1749,15 +1749,15 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="70" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="369" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1781,7 +1781,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1789,7 +1789,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="241" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1797,7 +1797,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1805,7 +1805,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="241" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1813,7 +1813,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1837,7 +1837,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1853,7 +1853,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1869,15 +1869,15 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="47" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="7" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1893,7 +1893,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1901,7 +1901,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1925,7 +1925,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1941,7 +1941,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1957,7 +1957,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1965,7 +1965,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
@@ -1973,7 +1973,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="11" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1981,15 +1981,15 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="70" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1997,7 +1997,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="4" t="s">
@@ -2005,7 +2005,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2013,7 +2013,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="11" t="s">
         <v>75</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2029,7 +2029,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="11" t="s">
         <v>77</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2037,7 +2037,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>79</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2045,7 +2045,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2061,7 +2061,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2069,7 +2069,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="11" t="s">
         <v>87</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2077,7 +2077,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="11" t="s">
         <v>89</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2085,7 +2085,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="11" t="s">
         <v>91</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2101,7 +2101,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="11" t="s">
         <v>95</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2109,7 +2109,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="11" t="s">
         <v>97</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2117,7 +2117,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -2125,7 +2125,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="11" t="s">
         <v>101</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2133,7 +2133,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="11" t="s">
         <v>103</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="11" t="s">
         <v>105</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2149,7 +2149,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="11" t="s">
         <v>107</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2157,7 +2157,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="11" t="s">
         <v>109</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="11" t="s">
         <v>111</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -2173,7 +2173,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -2181,7 +2181,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -2189,7 +2189,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2197,7 +2197,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="11" t="s">
         <v>119</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -2205,7 +2205,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="11" t="s">
         <v>121</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -2213,7 +2213,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="11" t="s">
         <v>123</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -2221,7 +2221,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+      <c r="A65" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="11" t="s">
         <v>127</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -2237,7 +2237,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" ht="193" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="11" t="s">
         <v>131</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -2253,7 +2253,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="225" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="11" t="s">
         <v>133</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -2261,7 +2261,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+      <c r="A70" s="11" t="s">
         <v>135</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -2269,7 +2269,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="11" t="s">
         <v>137</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2277,7 +2277,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+      <c r="A72" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -2285,7 +2285,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -2293,7 +2293,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="11" t="s">
         <v>143</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -2301,15 +2301,15 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="47" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="7" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
+      <c r="A76" s="11" t="s">
         <v>146</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -2317,7 +2317,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
+      <c r="A77" s="11" t="s">
         <v>148</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -2325,7 +2325,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
+      <c r="A78" s="11" t="s">
         <v>150</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -2333,7 +2333,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="11" t="s">
         <v>152</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -2341,7 +2341,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
+      <c r="A80" s="11" t="s">
         <v>154</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -2349,7 +2349,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="11" t="s">
         <v>156</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -2357,7 +2357,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" ht="193" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
+      <c r="A82" s="11" t="s">
         <v>158</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -2365,7 +2365,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
+      <c r="A83" s="11" t="s">
         <v>160</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -2373,7 +2373,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
+      <c r="A84" s="11" t="s">
         <v>162</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -2381,7 +2381,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
+      <c r="A85" s="11" t="s">
         <v>164</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -2389,7 +2389,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
+      <c r="A86" s="11" t="s">
         <v>166</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -2397,7 +2397,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" ht="161" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="11" t="s">
         <v>168</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -2405,7 +2405,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
+      <c r="A88" s="11" t="s">
         <v>170</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
+      <c r="A89" s="11" t="s">
         <v>172</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -2421,7 +2421,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
+      <c r="A90" s="11" t="s">
         <v>174</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -2429,7 +2429,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" ht="161" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
+      <c r="A91" s="11" t="s">
         <v>176</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -2437,7 +2437,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="11" t="s">
         <v>178</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -2445,15 +2445,15 @@
       </c>
     </row>
     <row r="93" spans="1:2" ht="47" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
+      <c r="A93" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="7" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
+      <c r="A94" s="11" t="s">
         <v>181</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -2461,7 +2461,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="11" t="s">
         <v>183</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -2469,7 +2469,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="11" t="s">
         <v>185</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -2477,7 +2477,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="11" t="s">
         <v>187</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -2485,7 +2485,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="13" t="s">
+      <c r="A98" s="11" t="s">
         <v>189</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -2493,7 +2493,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="13" t="s">
+      <c r="A99" s="11" t="s">
         <v>191</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -2501,7 +2501,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
+      <c r="A100" s="11" t="s">
         <v>193</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -2509,7 +2509,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="11" t="s">
         <v>195</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -2517,7 +2517,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
+      <c r="A102" s="11" t="s">
         <v>197</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
+      <c r="A103" s="11" t="s">
         <v>199</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -2533,7 +2533,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
+      <c r="A104" s="11" t="s">
         <v>201</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -2541,7 +2541,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="11" t="s">
         <v>203</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -2549,7 +2549,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
+      <c r="A106" s="11" t="s">
         <v>205</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -2557,7 +2557,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
+      <c r="A107" s="11" t="s">
         <v>207</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
+      <c r="A108" s="11" t="s">
         <v>209</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
+      <c r="A109" s="11" t="s">
         <v>211</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="s">
+      <c r="A110" s="11" t="s">
         <v>213</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="13" t="s">
+      <c r="A111" s="11" t="s">
         <v>215</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -2597,7 +2597,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="s">
+      <c r="A112" s="11" t="s">
         <v>217</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -2605,7 +2605,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" ht="161" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="s">
+      <c r="A113" s="11" t="s">
         <v>219</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -2613,7 +2613,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="s">
+      <c r="A114" s="11" t="s">
         <v>221</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -2621,7 +2621,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="s">
+      <c r="A115" s="11" t="s">
         <v>223</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="11" t="s">
         <v>225</v>
       </c>
       <c r="B116" s="3" t="s">
@@ -2637,7 +2637,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="s">
+      <c r="A117" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -2645,15 +2645,15 @@
       </c>
     </row>
     <row r="118" spans="1:2" ht="47" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
+      <c r="A118" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="7" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
+      <c r="A119" s="11" t="s">
         <v>230</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -2661,7 +2661,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="s">
+      <c r="A120" s="11" t="s">
         <v>232</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -2669,7 +2669,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="s">
+      <c r="A121" s="11" t="s">
         <v>234</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -2677,7 +2677,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="s">
+      <c r="A122" s="11" t="s">
         <v>236</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -2685,7 +2685,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="s">
+      <c r="A123" s="11" t="s">
         <v>238</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -2693,7 +2693,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="s">
+      <c r="A124" s="11" t="s">
         <v>240</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -2701,7 +2701,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="13" t="s">
+      <c r="A125" s="11" t="s">
         <v>242</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -2709,7 +2709,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="13" t="s">
+      <c r="A126" s="11" t="s">
         <v>244</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -2717,7 +2717,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="13" t="s">
+      <c r="A127" s="11" t="s">
         <v>246</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -2725,7 +2725,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="13" t="s">
+      <c r="A128" s="11" t="s">
         <v>248</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -2733,7 +2733,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
+      <c r="A129" s="11" t="s">
         <v>250</v>
       </c>
       <c r="B129" s="3" t="s">
@@ -2741,7 +2741,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="13" t="s">
+      <c r="A130" s="11" t="s">
         <v>252</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -2749,7 +2749,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="13" t="s">
+      <c r="A131" s="11" t="s">
         <v>254</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -2757,7 +2757,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="13" t="s">
+      <c r="A132" s="11" t="s">
         <v>256</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -2765,7 +2765,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="13" t="s">
+      <c r="A133" s="11" t="s">
         <v>258</v>
       </c>
       <c r="B133" s="3" t="s">
@@ -2773,7 +2773,7 @@
       </c>
     </row>
     <row r="134" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="13" t="s">
+      <c r="A134" s="11" t="s">
         <v>260</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -2781,7 +2781,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="13" t="s">
+      <c r="A135" s="11" t="s">
         <v>262</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -2789,7 +2789,7 @@
       </c>
     </row>
     <row r="136" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="13" t="s">
+      <c r="A136" s="11" t="s">
         <v>264</v>
       </c>
       <c r="B136" s="3" t="s">
@@ -2797,7 +2797,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="13" t="s">
+      <c r="A137" s="11" t="s">
         <v>266</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -2805,7 +2805,7 @@
       </c>
     </row>
     <row r="138" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="13" t="s">
+      <c r="A138" s="11" t="s">
         <v>268</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -2813,7 +2813,7 @@
       </c>
     </row>
     <row r="139" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="13" t="s">
+      <c r="A139" s="11" t="s">
         <v>270</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -2821,7 +2821,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="13" t="s">
+      <c r="A140" s="11" t="s">
         <v>272</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -2829,15 +2829,15 @@
       </c>
     </row>
     <row r="141" spans="1:2" ht="47" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14" t="s">
+      <c r="A141" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="B141" s="9" t="s">
+      <c r="B141" s="7" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="13" t="s">
+      <c r="A142" s="11" t="s">
         <v>275</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -2845,7 +2845,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="13" t="s">
+      <c r="A143" s="11" t="s">
         <v>277</v>
       </c>
       <c r="B143" s="3" t="s">
@@ -2853,7 +2853,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="13" t="s">
+      <c r="A144" s="11" t="s">
         <v>279</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -2861,7 +2861,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" ht="55" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="13" t="s">
+      <c r="A145" s="11" t="s">
         <v>281</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -2869,7 +2869,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="13" t="s">
+      <c r="A146" s="11" t="s">
         <v>283</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -2877,7 +2877,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" ht="145" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="13" t="s">
+      <c r="A147" s="11" t="s">
         <v>285</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -2885,7 +2885,7 @@
       </c>
     </row>
     <row r="148" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="13" t="s">
+      <c r="A148" s="11" t="s">
         <v>287</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -2893,7 +2893,7 @@
       </c>
     </row>
     <row r="149" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="13" t="s">
+      <c r="A149" s="11" t="s">
         <v>289</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -2901,7 +2901,7 @@
       </c>
     </row>
     <row r="150" spans="1:2" ht="193" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="13" t="s">
+      <c r="A150" s="11" t="s">
         <v>291</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -2909,7 +2909,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="13" t="s">
+      <c r="A151" s="11" t="s">
         <v>293</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -2917,7 +2917,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="13" t="s">
+      <c r="A152" s="11" t="s">
         <v>295</v>
       </c>
       <c r="B152" s="3" t="s">
@@ -2925,7 +2925,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="13" t="s">
+      <c r="A153" s="11" t="s">
         <v>297</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -2933,7 +2933,7 @@
       </c>
     </row>
     <row r="154" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="13" t="s">
+      <c r="A154" s="11" t="s">
         <v>299</v>
       </c>
       <c r="B154" s="3" t="s">
@@ -2941,7 +2941,7 @@
       </c>
     </row>
     <row r="155" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="13" t="s">
+      <c r="A155" s="11" t="s">
         <v>301</v>
       </c>
       <c r="B155" s="3" t="s">
@@ -2949,7 +2949,7 @@
       </c>
     </row>
     <row r="156" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="13" t="s">
+      <c r="A156" s="11" t="s">
         <v>303</v>
       </c>
       <c r="B156" s="3" t="s">
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="157" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="13" t="s">
+      <c r="A157" s="11" t="s">
         <v>305</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -2965,7 +2965,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="13" t="s">
+      <c r="A158" s="11" t="s">
         <v>307</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -2973,7 +2973,7 @@
       </c>
     </row>
     <row r="159" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="13" t="s">
+      <c r="A159" s="11" t="s">
         <v>309</v>
       </c>
       <c r="B159" s="3" t="s">
@@ -2981,7 +2981,7 @@
       </c>
     </row>
     <row r="160" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="13" t="s">
+      <c r="A160" s="11" t="s">
         <v>311</v>
       </c>
       <c r="B160" s="5" t="s">
@@ -2989,7 +2989,7 @@
       </c>
     </row>
     <row r="161" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="13" t="s">
+      <c r="A161" s="11" t="s">
         <v>313</v>
       </c>
       <c r="B161" s="5" t="s">
@@ -2997,7 +2997,7 @@
       </c>
     </row>
     <row r="162" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="13" t="s">
+      <c r="A162" s="11" t="s">
         <v>315</v>
       </c>
       <c r="B162" s="3" t="s">
@@ -3005,19 +3005,19 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" s="15" t="s">
+      <c r="A163" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="16" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="16"/>
-      <c r="B164" s="7"/>
+      <c r="A164" s="15"/>
+      <c r="B164" s="17"/>
     </row>
     <row r="165" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="13" t="s">
+      <c r="A165" s="11" t="s">
         <v>319</v>
       </c>
       <c r="B165" s="3" t="s">
@@ -3025,7 +3025,7 @@
       </c>
     </row>
     <row r="166" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="13" t="s">
+      <c r="A166" s="11" t="s">
         <v>321</v>
       </c>
       <c r="B166" s="3" t="s">
@@ -3033,7 +3033,7 @@
       </c>
     </row>
     <row r="167" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="13" t="s">
+      <c r="A167" s="11" t="s">
         <v>323</v>
       </c>
       <c r="B167" s="3" t="s">
@@ -3041,7 +3041,7 @@
       </c>
     </row>
     <row r="168" spans="1:2" ht="161" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="13" t="s">
+      <c r="A168" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -3049,7 +3049,7 @@
       </c>
     </row>
     <row r="169" spans="1:2" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="13" t="s">
+      <c r="A169" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B169" s="3" t="s">
@@ -3057,7 +3057,7 @@
       </c>
     </row>
     <row r="170" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="13" t="s">
+      <c r="A170" s="11" t="s">
         <v>329</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -3065,7 +3065,7 @@
       </c>
     </row>
     <row r="171" spans="1:2" ht="161" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="13" t="s">
+      <c r="A171" s="11" t="s">
         <v>331</v>
       </c>
       <c r="B171" s="3" t="s">
@@ -3073,7 +3073,7 @@
       </c>
     </row>
     <row r="172" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="13" t="s">
+      <c r="A172" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B172" s="3" t="s">
@@ -3081,7 +3081,7 @@
       </c>
     </row>
     <row r="173" spans="1:2" ht="37" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="13" t="s">
+      <c r="A173" s="11" t="s">
         <v>335</v>
       </c>
       <c r="B173" s="3" t="s">
@@ -3089,7 +3089,7 @@
       </c>
     </row>
     <row r="174" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="13" t="s">
+      <c r="A174" s="11" t="s">
         <v>337</v>
       </c>
       <c r="B174" s="3" t="s">
@@ -3097,7 +3097,7 @@
       </c>
     </row>
     <row r="175" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="13" t="s">
+      <c r="A175" s="11" t="s">
         <v>339</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="176" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="13" t="s">
+      <c r="A176" s="11" t="s">
         <v>341</v>
       </c>
       <c r="B176" s="3" t="s">
@@ -3113,15 +3113,15 @@
       </c>
     </row>
     <row r="177" spans="1:2" ht="70" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14" t="s">
+      <c r="A177" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="B177" s="9" t="s">
+      <c r="B177" s="7" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="13" t="s">
+      <c r="A178" s="11" t="s">
         <v>344</v>
       </c>
       <c r="B178" s="3" t="s">
@@ -3129,7 +3129,7 @@
       </c>
     </row>
     <row r="179" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="13" t="s">
+      <c r="A179" s="11" t="s">
         <v>346</v>
       </c>
       <c r="B179" s="3" t="s">
@@ -3137,7 +3137,7 @@
       </c>
     </row>
     <row r="180" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="13" t="s">
+      <c r="A180" s="11" t="s">
         <v>348</v>
       </c>
       <c r="B180" s="3" t="s">
@@ -3145,7 +3145,7 @@
       </c>
     </row>
     <row r="181" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="13" t="s">
+      <c r="A181" s="11" t="s">
         <v>350</v>
       </c>
       <c r="B181" s="3" t="s">
@@ -3153,7 +3153,7 @@
       </c>
     </row>
     <row r="182" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="13" t="s">
+      <c r="A182" s="11" t="s">
         <v>352</v>
       </c>
       <c r="B182" s="3" t="s">
@@ -3161,7 +3161,7 @@
       </c>
     </row>
     <row r="183" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="13" t="s">
+      <c r="A183" s="11" t="s">
         <v>354</v>
       </c>
       <c r="B183" s="3" t="s">
@@ -3169,7 +3169,7 @@
       </c>
     </row>
     <row r="184" spans="1:2" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="13" t="s">
+      <c r="A184" s="11" t="s">
         <v>356</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -3177,7 +3177,7 @@
       </c>
     </row>
     <row r="185" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="13" t="s">
+      <c r="A185" s="11" t="s">
         <v>358</v>
       </c>
       <c r="B185" s="3" t="s">
@@ -3185,7 +3185,7 @@
       </c>
     </row>
     <row r="186" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="13" t="s">
+      <c r="A186" s="11" t="s">
         <v>360</v>
       </c>
       <c r="B186" s="3" t="s">
@@ -3193,7 +3193,7 @@
       </c>
     </row>
     <row r="187" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="13" t="s">
+      <c r="A187" s="11" t="s">
         <v>362</v>
       </c>
       <c r="B187" s="3" t="s">
@@ -3201,7 +3201,7 @@
       </c>
     </row>
     <row r="188" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="13" t="s">
+      <c r="A188" s="11" t="s">
         <v>364</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -3209,7 +3209,7 @@
       </c>
     </row>
     <row r="189" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="13" t="s">
+      <c r="A189" s="11" t="s">
         <v>366</v>
       </c>
       <c r="B189" s="3" t="s">
@@ -3217,7 +3217,7 @@
       </c>
     </row>
     <row r="190" spans="1:2" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="13" t="s">
+      <c r="A190" s="11" t="s">
         <v>368</v>
       </c>
       <c r="B190" s="3" t="s">
@@ -3225,7 +3225,7 @@
       </c>
     </row>
     <row r="191" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="13" t="s">
+      <c r="A191" s="11" t="s">
         <v>370</v>
       </c>
       <c r="B191" s="3" t="s">
@@ -3233,7 +3233,7 @@
       </c>
     </row>
     <row r="192" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="13" t="s">
+      <c r="A192" s="11" t="s">
         <v>372</v>
       </c>
       <c r="B192" s="3" t="s">
@@ -3241,7 +3241,7 @@
       </c>
     </row>
     <row r="193" spans="1:2" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="13" t="s">
+      <c r="A193" s="11" t="s">
         <v>374</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="194" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="13" t="s">
+      <c r="A194" s="11" t="s">
         <v>376</v>
       </c>
       <c r="B194" s="3" t="s">
@@ -3257,7 +3257,7 @@
       </c>
     </row>
     <row r="195" spans="1:2" ht="177" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="13" t="s">
+      <c r="A195" s="11" t="s">
         <v>378</v>
       </c>
       <c r="B195" s="3" t="s">
@@ -3265,7 +3265,7 @@
       </c>
     </row>
     <row r="196" spans="1:2" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="13" t="s">
+      <c r="A196" s="11" t="s">
         <v>380</v>
       </c>
       <c r="B196" s="3" t="s">
@@ -3273,7 +3273,7 @@
       </c>
     </row>
     <row r="197" spans="1:2" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="13" t="s">
+      <c r="A197" s="11" t="s">
         <v>382</v>
       </c>
       <c r="B197" s="3" t="s">
@@ -3281,7 +3281,7 @@
       </c>
     </row>
     <row r="198" spans="1:2" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="13" t="s">
+      <c r="A198" s="11" t="s">
         <v>384</v>
       </c>
       <c r="B198" s="3" t="s">
@@ -3289,7 +3289,7 @@
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A199" s="17"/>
+      <c r="A199" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>